<commit_message>
Finished Day2 cleaning and pre-processing
</commit_message>
<xml_diff>
--- a/Day2/covid_dataset.xlsx
+++ b/Day2/covid_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dg519/Documents/Computational-Methods-for-the-Brain-Sciences/Day2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B14090-1AE5-2049-BB08-E9AAA2640621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23F638B-5DF5-DC42-BD84-7F2E4F4F9E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,7 +474,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -531,7 +531,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -840,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="223" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="BC7" workbookViewId="0">
+      <selection activeCell="BQ22" sqref="BQ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4852,7 +4852,7 @@
         <v>21</v>
       </c>
       <c r="BP17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BQ17">
         <v>57</v>

</xml_diff>